<commit_message>
Assay to Dataset, v1.3
</commit_message>
<xml_diff>
--- a/test/excel/SNP_vcf_test1.xlsx
+++ b/test/excel/SNP_vcf_test1.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19152" windowHeight="8208" firstSheet="3" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="11820" firstSheet="4" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="README" sheetId="1" r:id="rId1"/>
@@ -21,8 +21,8 @@
     <sheet name="Sample HELP" sheetId="27" r:id="rId7"/>
     <sheet name="Experiment" sheetId="12" r:id="rId8"/>
     <sheet name="Experiment HELP" sheetId="13" r:id="rId9"/>
-    <sheet name="Assay" sheetId="14" r:id="rId10"/>
-    <sheet name="Assay HELP" sheetId="15" r:id="rId11"/>
+    <sheet name="Dataset" sheetId="14" r:id="rId10"/>
+    <sheet name="Dataset HELP" sheetId="15" r:id="rId11"/>
     <sheet name="Variant Call (SV)" sheetId="22" r:id="rId12"/>
     <sheet name="Variant Call HELP" sheetId="23" r:id="rId13"/>
     <sheet name="Variant Region (SV)" sheetId="24" r:id="rId14"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="526">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="527">
   <si>
     <t>Placement</t>
   </si>
@@ -666,19 +666,11 @@
     <phoneticPr fontId="3"/>
   </si>
   <si>
-    <t>Assay ID</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
     <t>SampleSet ID</t>
     <phoneticPr fontId="3"/>
   </si>
   <si>
     <t>Experiment ID</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t>Assay Description</t>
     <phoneticPr fontId="3"/>
   </si>
   <si>
@@ -1561,10 +1553,6 @@
   </si>
   <si>
     <t>## An Assay references 1 SampleSet and 1 Experiment, and resulting variations in 1 VCF file or in Variant Call/Region sheets (for structural variations only).</t>
-    <phoneticPr fontId="3"/>
-  </si>
-  <si>
-    <t># Assay ID</t>
     <phoneticPr fontId="3"/>
   </si>
   <si>
@@ -2156,6 +2144,22 @@
   </si>
   <si>
     <t>control</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Dataset ID</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Dataset Description</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t># Dataset ID</t>
+    <phoneticPr fontId="3"/>
+  </si>
+  <si>
+    <t>Dataset Description</t>
     <phoneticPr fontId="3"/>
   </si>
 </sst>
@@ -3025,7 +3029,7 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>261</v>
+        <v>259</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
@@ -3033,17 +3037,17 @@
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" s="39" t="s">
-        <v>262</v>
+        <v>260</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" s="39" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" s="39" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
@@ -3051,78 +3055,78 @@
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>254</v>
+        <v>252</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>251</v>
+        <v>249</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>248</v>
+        <v>246</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="45" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>252</v>
+        <v>250</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>253</v>
+        <v>251</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="22" t="s">
-        <v>249</v>
+        <v>247</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A18" s="4" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
     </row>
     <row r="19" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
     </row>
     <row r="20" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>250</v>
+        <v>248</v>
       </c>
     </row>
     <row r="22" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="44" t="s">
-        <v>255</v>
+        <v>253</v>
       </c>
       <c r="C22" s="38"/>
       <c r="D22" s="38"/>
@@ -3152,7 +3156,7 @@
     <row r="23" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A23" s="3"/>
       <c r="B23" s="44" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="C23" s="38"/>
       <c r="D23" s="38"/>
@@ -3182,7 +3186,7 @@
     <row r="24" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
       <c r="B24" s="44" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C24" s="38"/>
       <c r="D24" s="38"/>
@@ -3212,7 +3216,7 @@
     <row r="25" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A25" s="68"/>
       <c r="B25" s="44" t="s">
-        <v>257</v>
+        <v>255</v>
       </c>
       <c r="C25" s="38"/>
       <c r="D25" s="38"/>
@@ -3272,7 +3276,7 @@
         <v>1</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C27" s="38"/>
       <c r="D27" s="38"/>
@@ -3327,7 +3331,7 @@
     </row>
     <row r="29" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A29" s="42" t="s">
-        <v>259</v>
+        <v>257</v>
       </c>
       <c r="B29" s="42">
         <v>45087</v>
@@ -3359,10 +3363,10 @@
     </row>
     <row r="30" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A30" s="43" t="s">
-        <v>260</v>
+        <v>258</v>
       </c>
       <c r="B30" s="43" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
       <c r="C30" s="38"/>
       <c r="D30" s="38"/>
@@ -3419,7 +3423,7 @@
     </row>
     <row r="32" spans="1:26" ht="262.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="40" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
       <c r="B32" s="38"/>
       <c r="C32" s="38"/>
@@ -30057,8 +30061,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G1003"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -30077,35 +30081,35 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="20" t="s">
-        <v>400</v>
+        <v>525</v>
       </c>
       <c r="B4" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="C4" s="17" t="s">
         <v>201</v>
       </c>
-      <c r="C4" s="17" t="s">
+      <c r="D4" s="18" t="s">
+        <v>245</v>
+      </c>
+      <c r="E4" s="17" t="s">
+        <v>526</v>
+      </c>
+      <c r="F4" s="19" t="s">
         <v>202</v>
       </c>
-      <c r="D4" s="18" t="s">
-        <v>247</v>
-      </c>
-      <c r="E4" s="17" t="s">
-        <v>203</v>
-      </c>
-      <c r="F4" s="19" t="s">
-        <v>204</v>
-      </c>
       <c r="G4" s="71" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -30122,11 +30126,11 @@
         <v>92</v>
       </c>
       <c r="E5" s="11" t="s">
-        <v>515</v>
+        <v>512</v>
       </c>
       <c r="F5" s="11"/>
       <c r="G5" s="11" t="s">
-        <v>516</v>
+        <v>513</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -30143,11 +30147,11 @@
         <v>92</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>523</v>
+        <v>520</v>
       </c>
       <c r="F6" s="11"/>
       <c r="G6" s="11" t="s">
-        <v>524</v>
+        <v>521</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -31242,7 +31246,7 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.59765625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -31266,15 +31270,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>401</v>
+        <v>398</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="47" t="s">
-        <v>200</v>
+        <v>523</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -31282,7 +31286,7 @@
         <v>174</v>
       </c>
       <c r="B4" s="46" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -31290,39 +31294,39 @@
         <v>186</v>
       </c>
       <c r="B5" s="46" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="54" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="B6" s="46" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>203</v>
+        <v>524</v>
       </c>
       <c r="B7" s="46" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="B8" s="46" t="s">
-        <v>307</v>
+        <v>305</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A9" s="72" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B9" s="46" t="s">
-        <v>489</v>
+        <v>486</v>
       </c>
     </row>
   </sheetData>
@@ -31340,7 +31344,7 @@
   <dimension ref="A1:AJ104"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.796875" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -31386,17 +31390,17 @@
   <sheetData>
     <row r="1" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>402</v>
+        <v>399</v>
       </c>
     </row>
     <row r="2" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
     </row>
     <row r="4" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A4" s="35" t="s">
-        <v>403</v>
+        <v>400</v>
       </c>
       <c r="B4" s="35"/>
       <c r="C4" s="35"/>
@@ -31414,7 +31418,7 @@
       <c r="M4" s="31"/>
       <c r="N4" s="36"/>
       <c r="O4" s="28" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="P4" s="31"/>
       <c r="Q4" s="31"/>
@@ -31428,7 +31432,7 @@
       <c r="Y4" s="31"/>
       <c r="Z4" s="36"/>
       <c r="AA4" s="28" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="AB4" s="31"/>
       <c r="AC4" s="31"/>
@@ -31442,10 +31446,10 @@
     </row>
     <row r="5" spans="1:36" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>404</v>
+        <v>401</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>185</v>
@@ -31457,97 +31461,97 @@
         <v>86</v>
       </c>
       <c r="F5" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="G5" s="8" t="s">
+        <v>207</v>
+      </c>
+      <c r="H5" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="G5" s="8" t="s">
+      <c r="I5" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="H5" s="8" t="s">
+      <c r="J5" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="I5" s="8" t="s">
+      <c r="K5" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="J5" s="8" t="s">
+      <c r="L5" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="K5" s="8" t="s">
+      <c r="M5" s="8" t="s">
         <v>213</v>
       </c>
-      <c r="L5" s="8" t="s">
+      <c r="N5" s="8" t="s">
         <v>214</v>
       </c>
-      <c r="M5" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="N5" s="8" t="s">
-        <v>216</v>
-      </c>
       <c r="O5" s="10" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="P5" s="10" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="Q5" s="10" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="R5" s="10" t="s">
+        <v>218</v>
+      </c>
+      <c r="S5" s="10" t="s">
+        <v>219</v>
+      </c>
+      <c r="T5" s="10" t="s">
         <v>220</v>
       </c>
-      <c r="S5" s="10" t="s">
+      <c r="U5" s="10" t="s">
         <v>221</v>
-      </c>
-      <c r="T5" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="U5" s="10" t="s">
-        <v>223</v>
       </c>
       <c r="V5" s="10" t="s">
         <v>83</v>
       </c>
       <c r="W5" s="10" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="X5" s="10" t="s">
         <v>198</v>
       </c>
       <c r="Y5" s="10" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z5" s="10" t="s">
+        <v>224</v>
+      </c>
+      <c r="AA5" s="8" t="s">
+        <v>459</v>
+      </c>
+      <c r="AB5" s="8" t="s">
         <v>225</v>
       </c>
-      <c r="Z5" s="10" t="s">
+      <c r="AC5" s="8" t="s">
         <v>226</v>
       </c>
-      <c r="AA5" s="8" t="s">
-        <v>462</v>
-      </c>
-      <c r="AB5" s="8" t="s">
+      <c r="AD5" s="8" t="s">
         <v>227</v>
       </c>
-      <c r="AC5" s="8" t="s">
+      <c r="AE5" s="8" t="s">
         <v>228</v>
       </c>
-      <c r="AD5" s="8" t="s">
+      <c r="AF5" s="8" t="s">
         <v>229</v>
       </c>
-      <c r="AE5" s="8" t="s">
+      <c r="AG5" s="8" t="s">
         <v>230</v>
       </c>
-      <c r="AF5" s="8" t="s">
+      <c r="AH5" s="8" t="s">
         <v>231</v>
       </c>
-      <c r="AG5" s="8" t="s">
+      <c r="AI5" s="8" t="s">
         <v>232</v>
       </c>
-      <c r="AH5" s="8" t="s">
+      <c r="AJ5" s="8" t="s">
         <v>233</v>
-      </c>
-      <c r="AI5" s="8" t="s">
-        <v>234</v>
-      </c>
-      <c r="AJ5" s="8" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="6" spans="1:36" x14ac:dyDescent="0.25">
@@ -35367,32 +35371,32 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="67" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="73" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="B4" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C4" s="46" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="74"/>
       <c r="B5" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C5" s="46" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -35401,7 +35405,7 @@
         <v>185</v>
       </c>
       <c r="C6" s="46" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -35410,7 +35414,7 @@
         <v>173</v>
       </c>
       <c r="C7" s="46" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -35418,12 +35422,12 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="51" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="52" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -35437,78 +35441,78 @@
         <v>86</v>
       </c>
       <c r="C12" s="46" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="74"/>
       <c r="B13" s="8" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C13" s="46" t="s">
-        <v>298</v>
+        <v>296</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="74"/>
       <c r="B14" s="8" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C14" s="46" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="74"/>
       <c r="B15" s="8" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C15" s="75" t="s">
-        <v>299</v>
+        <v>297</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="74"/>
       <c r="B16" s="8" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C16" s="75"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="74"/>
       <c r="B17" s="8" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C17" s="75"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="74"/>
       <c r="B18" s="8" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C18" s="75"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="74"/>
       <c r="B19" s="8" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C19" s="75"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="74"/>
       <c r="B20" s="8" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C20" s="75"/>
     </row>
     <row r="21" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A21" s="74"/>
       <c r="B21" s="8" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="C21" s="46" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -35517,64 +35521,64 @@
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="74"/>
       <c r="B23" s="10" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C23" s="46" t="s">
-        <v>303</v>
+        <v>301</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="74"/>
       <c r="B24" s="10" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C24" s="46" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="74"/>
       <c r="B25" s="10" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C25" s="46" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="74"/>
       <c r="B26" s="10" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C26" s="46" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="74"/>
       <c r="B27" s="10" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C27" s="46" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A28" s="74"/>
       <c r="B28" s="10" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C28" s="46" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="74"/>
       <c r="B29" s="10" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C29" s="46" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
@@ -35583,16 +35587,16 @@
         <v>83</v>
       </c>
       <c r="C30" s="46" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="74"/>
       <c r="B31" s="10" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C31" s="46" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
@@ -35601,25 +35605,25 @@
         <v>198</v>
       </c>
       <c r="C32" s="46" t="s">
-        <v>306</v>
+        <v>304</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="74"/>
       <c r="B33" s="10" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C33" s="46" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A34" s="74"/>
       <c r="B34" s="10" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="C34" s="46" t="s">
-        <v>305</v>
+        <v>303</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
@@ -35627,75 +35631,75 @@
     </row>
     <row r="36" spans="1:3" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="73" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>462</v>
+        <v>459</v>
       </c>
       <c r="C36" s="75" t="s">
-        <v>308</v>
+        <v>306</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="74"/>
       <c r="B37" s="8" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="C37" s="75"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="74"/>
       <c r="B38" s="8" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="C38" s="75"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="74"/>
       <c r="B39" s="8" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="C39" s="75"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="74"/>
       <c r="B40" s="8" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="C40" s="75"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="74"/>
       <c r="B41" s="8" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C41" s="75"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="74"/>
       <c r="B42" s="8" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="C42" s="75"/>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="74"/>
       <c r="B43" s="8" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C43" s="75"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="74"/>
       <c r="B44" s="8" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="C44" s="75"/>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="74"/>
       <c r="B45" s="8" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="C45" s="75"/>
     </row>
@@ -35744,22 +35748,22 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" s="28" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="B4" s="29"/>
       <c r="C4" s="30"/>
       <c r="D4" s="31" t="s">
-        <v>312</v>
+        <v>310</v>
       </c>
       <c r="E4" s="29"/>
       <c r="F4" s="29"/>
@@ -35770,56 +35774,56 @@
       <c r="K4" s="29"/>
       <c r="L4" s="30"/>
       <c r="M4" s="31" t="s">
-        <v>313</v>
+        <v>311</v>
       </c>
       <c r="N4" s="29"/>
       <c r="O4" s="30"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="B5" s="33" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C5" s="33" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="D5" s="34" t="s">
         <v>86</v>
       </c>
       <c r="E5" s="34" t="s">
+        <v>206</v>
+      </c>
+      <c r="F5" s="34" t="s">
+        <v>207</v>
+      </c>
+      <c r="G5" s="34" t="s">
         <v>208</v>
       </c>
-      <c r="F5" s="34" t="s">
+      <c r="H5" s="34" t="s">
         <v>209</v>
       </c>
-      <c r="G5" s="34" t="s">
+      <c r="I5" s="34" t="s">
         <v>210</v>
       </c>
-      <c r="H5" s="34" t="s">
+      <c r="J5" s="34" t="s">
         <v>211</v>
       </c>
-      <c r="I5" s="34" t="s">
+      <c r="K5" s="34" t="s">
         <v>212</v>
       </c>
-      <c r="J5" s="34" t="s">
+      <c r="L5" s="34" t="s">
         <v>213</v>
       </c>
-      <c r="K5" s="34" t="s">
-        <v>214</v>
-      </c>
-      <c r="L5" s="34" t="s">
-        <v>215</v>
-      </c>
       <c r="M5" s="34" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="N5" s="37" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="O5" s="37" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -37558,41 +37562,41 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="67" t="s">
-        <v>412</v>
+        <v>409</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="76" t="s">
-        <v>314</v>
+        <v>312</v>
       </c>
       <c r="B4" s="33" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C4" s="56" t="s">
-        <v>309</v>
+        <v>307</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="77"/>
       <c r="B5" s="33" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="C5" s="56" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="55.2" x14ac:dyDescent="0.25">
       <c r="A6" s="77"/>
       <c r="B6" s="33" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="C6" s="46" t="s">
-        <v>311</v>
+        <v>309</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -37600,104 +37604,104 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="76" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="B8" s="34" t="s">
         <v>86</v>
       </c>
       <c r="C8" s="56" t="s">
-        <v>310</v>
+        <v>308</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="77"/>
       <c r="B9" s="34" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C9" s="46" t="s">
-        <v>317</v>
+        <v>315</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A10" s="77"/>
       <c r="B10" s="34" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C10" s="56" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="77"/>
       <c r="B11" s="34" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C11" s="78" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="77"/>
       <c r="B12" s="34" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="C12" s="79"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="77"/>
       <c r="B13" s="34" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C13" s="79"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="77"/>
       <c r="B14" s="34" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C14" s="79"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="77"/>
       <c r="B15" s="34" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="C15" s="79"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="77"/>
       <c r="B16" s="34" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C16" s="80"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="76" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="B18" s="34" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C18" s="46" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="27.6" x14ac:dyDescent="0.25">
       <c r="A19" s="77"/>
       <c r="B19" s="37" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="C19" s="46" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="77"/>
       <c r="B20" s="37" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C20" s="56" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -37734,7 +37738,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -38110,46 +38114,46 @@
   <sheetData>
     <row r="1" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
+        <v>241</v>
+      </c>
+      <c r="B1" s="22" t="s">
+        <v>242</v>
+      </c>
+      <c r="C1" s="22" t="s">
+        <v>356</v>
+      </c>
+      <c r="D1" s="22" t="s">
+        <v>357</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>358</v>
+      </c>
+      <c r="F1" s="22" t="s">
+        <v>455</v>
+      </c>
+      <c r="G1" s="22" t="s">
+        <v>377</v>
+      </c>
+      <c r="H1" s="22" t="s">
+        <v>378</v>
+      </c>
+      <c r="I1" s="22" t="s">
+        <v>379</v>
+      </c>
+      <c r="J1" s="22" t="s">
         <v>243</v>
       </c>
-      <c r="B1" s="22" t="s">
+      <c r="K1" s="22" t="s">
         <v>244</v>
       </c>
-      <c r="C1" s="22" t="s">
-        <v>358</v>
-      </c>
-      <c r="D1" s="22" t="s">
-        <v>359</v>
-      </c>
-      <c r="E1" s="22" t="s">
-        <v>360</v>
-      </c>
-      <c r="F1" s="22" t="s">
-        <v>458</v>
-      </c>
-      <c r="G1" s="22" t="s">
-        <v>379</v>
-      </c>
-      <c r="H1" s="22" t="s">
-        <v>380</v>
-      </c>
-      <c r="I1" s="22" t="s">
-        <v>381</v>
-      </c>
-      <c r="J1" s="22" t="s">
-        <v>245</v>
-      </c>
-      <c r="K1" s="22" t="s">
-        <v>246</v>
-      </c>
       <c r="L1" s="22" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="M1" s="22" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="N1" s="22" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="O1" s="22"/>
     </row>
@@ -38164,13 +38168,13 @@
         <v>88</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>351</v>
+        <v>349</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="G2" s="4" t="s">
         <v>85</v>
@@ -38188,13 +38192,13 @@
         <v>91</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="M2" s="4" t="s">
         <v>90</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -38208,13 +38212,13 @@
         <v>95</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>352</v>
+        <v>350</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="G3" s="4" t="s">
         <v>92</v>
@@ -38232,13 +38236,13 @@
         <v>98</v>
       </c>
       <c r="L3" s="4" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="M3" s="4" t="s">
         <v>99</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -38249,13 +38253,13 @@
         <v>103</v>
       </c>
       <c r="D4" s="4" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="G4" s="4" t="s">
         <v>101</v>
@@ -38273,13 +38277,13 @@
         <v>105</v>
       </c>
       <c r="L4" s="4" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="M4" s="4" t="s">
         <v>106</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -38287,10 +38291,10 @@
         <v>110</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>354</v>
+        <v>352</v>
       </c>
       <c r="G5" s="4" t="s">
         <v>108</v>
@@ -38305,7 +38309,7 @@
         <v>106</v>
       </c>
       <c r="L5" s="4" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="M5" s="4" t="s">
         <v>111</v>
@@ -38316,10 +38320,10 @@
         <v>115</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>113</v>
@@ -38334,7 +38338,7 @@
         <v>116</v>
       </c>
       <c r="L6" s="4" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="M6" s="4" t="s">
         <v>117</v>
@@ -38345,10 +38349,10 @@
         <v>120</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>348</v>
+        <v>346</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>119</v>
@@ -38360,7 +38364,7 @@
         <v>121</v>
       </c>
       <c r="L7" s="4" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="M7" s="4" t="s">
         <v>122</v>
@@ -38368,10 +38372,10 @@
     </row>
     <row r="8" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" s="4" t="s">
-        <v>349</v>
+        <v>347</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>124</v>
@@ -38383,7 +38387,7 @@
         <v>111</v>
       </c>
       <c r="L8" s="4" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="M8" s="4" t="s">
         <v>125</v>
@@ -38391,7 +38395,7 @@
     </row>
     <row r="9" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D9" s="4" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="G9" s="4" t="s">
         <v>127</v>
@@ -38403,7 +38407,7 @@
         <v>117</v>
       </c>
       <c r="L9" s="4" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="M9" s="4" t="s">
         <v>128</v>
@@ -38420,7 +38424,7 @@
         <v>130</v>
       </c>
       <c r="L10" s="4" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="M10" s="4" t="s">
         <v>131</v>
@@ -38437,7 +38441,7 @@
         <v>134</v>
       </c>
       <c r="L11" s="4" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="M11" s="4" t="s">
         <v>135</v>
@@ -38454,7 +38458,7 @@
         <v>122</v>
       </c>
       <c r="L12" s="4" t="s">
-        <v>481</v>
+        <v>478</v>
       </c>
       <c r="M12" s="4" t="s">
         <v>138</v>
@@ -38471,7 +38475,7 @@
         <v>125</v>
       </c>
       <c r="L13" s="4" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
       <c r="M13" s="4" t="s">
         <v>140</v>
@@ -38488,7 +38492,7 @@
         <v>143</v>
       </c>
       <c r="L14" s="4" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="M14" s="4" t="s">
         <v>144</v>
@@ -38505,7 +38509,7 @@
         <v>146</v>
       </c>
       <c r="L15" s="4" t="s">
-        <v>484</v>
+        <v>481</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -38519,7 +38523,7 @@
         <v>149</v>
       </c>
       <c r="L16" s="4" t="s">
-        <v>485</v>
+        <v>482</v>
       </c>
     </row>
     <row r="17" spans="7:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -38533,7 +38537,7 @@
         <v>152</v>
       </c>
       <c r="L17" s="4" t="s">
-        <v>486</v>
+        <v>483</v>
       </c>
     </row>
     <row r="18" spans="7:12" ht="18" customHeight="1" x14ac:dyDescent="0.25">
@@ -39597,7 +39601,7 @@
   <dimension ref="A1:F1008"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="23.09765625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -39607,21 +39611,21 @@
   <sheetData>
     <row r="1" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -39629,15 +39633,15 @@
         <v>167</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
@@ -39646,7 +39650,7 @@
     </row>
     <row r="7" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -39656,10 +39660,10 @@
     </row>
     <row r="8" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -39668,10 +39672,10 @@
     </row>
     <row r="9" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
@@ -39680,10 +39684,10 @@
     </row>
     <row r="10" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
@@ -39692,10 +39696,10 @@
     </row>
     <row r="11" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B11" s="63" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -39703,7 +39707,7 @@
         <v>169</v>
       </c>
       <c r="B12" s="63" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -39733,7 +39737,7 @@
         <v>182</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>507</v>
+        <v>504</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -39753,12 +39757,12 @@
         <v>168</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>508</v>
+        <v>505</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="69" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="B20" s="70">
         <v>45017</v>
@@ -39766,19 +39770,19 @@
     </row>
     <row r="21" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="69" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="B21" s="70"/>
     </row>
     <row r="22" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="69" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="B22" s="70"/>
     </row>
     <row r="23" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="69" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="B23" s="6"/>
     </row>
@@ -40810,16 +40814,16 @@
   <sheetData>
     <row r="1" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>423</v>
+        <v>420</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>426</v>
+        <v>423</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -40827,55 +40831,55 @@
         <v>167</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>446</v>
+        <v>443</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>416</v>
+        <v>413</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>413</v>
+        <v>410</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -40883,7 +40887,7 @@
         <v>169</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
     </row>
     <row r="12" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -40891,7 +40895,7 @@
         <v>170</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="13" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -40899,7 +40903,7 @@
         <v>184</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
     </row>
     <row r="14" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -40907,7 +40911,7 @@
         <v>183</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
     </row>
     <row r="15" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -40915,7 +40919,7 @@
         <v>182</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -40923,7 +40927,7 @@
         <v>171</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -40931,7 +40935,7 @@
         <v>172</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -40939,39 +40943,39 @@
         <v>168</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>440</v>
+        <v>437</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="69" t="s">
-        <v>418</v>
+        <v>415</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="69" t="s">
-        <v>419</v>
+        <v>416</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>442</v>
+        <v>439</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="69" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
     </row>
     <row r="22" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="69" t="s">
-        <v>421</v>
+        <v>418</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>444</v>
+        <v>441</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="17.25" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -41973,7 +41977,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -41992,19 +41996,19 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="C1" s="22"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C2" s="22"/>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="9" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>175</v>
@@ -42039,7 +42043,7 @@
         <v>87</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="E5" s="6"/>
       <c r="F5" s="6"/>
@@ -42056,10 +42060,10 @@
         <v>2</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>525</v>
+        <v>522</v>
       </c>
       <c r="E6" s="6"/>
       <c r="F6" s="6"/>
@@ -42147,7 +42151,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -42155,7 +42159,7 @@
         <v>174</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -42163,7 +42167,7 @@
         <v>175</v>
       </c>
       <c r="B4" s="46" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
@@ -42171,7 +42175,7 @@
         <v>176</v>
       </c>
       <c r="B5" s="46" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
@@ -42179,7 +42183,7 @@
         <v>177</v>
       </c>
       <c r="B6" s="46" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -42187,7 +42191,7 @@
         <v>178</v>
       </c>
       <c r="B7" s="46" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="41.4" x14ac:dyDescent="0.25">
@@ -42195,7 +42199,7 @@
         <v>179</v>
       </c>
       <c r="B8" s="46" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
@@ -42203,7 +42207,7 @@
         <v>180</v>
       </c>
       <c r="B9" s="46" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
@@ -42211,7 +42215,7 @@
         <v>181</v>
       </c>
       <c r="B10" s="46" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
   </sheetData>
@@ -42253,30 +42257,30 @@
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="B1" s="22"/>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
     </row>
     <row r="4" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A4" s="58" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="B4" s="59"/>
       <c r="C4" s="59"/>
       <c r="D4" s="36"/>
       <c r="E4" s="58" t="s">
-        <v>328</v>
+        <v>326</v>
       </c>
       <c r="F4" s="59"/>
       <c r="G4" s="59"/>
       <c r="H4" s="31"/>
       <c r="I4" s="28" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="J4" s="31"/>
       <c r="K4" s="31"/>
@@ -42289,66 +42293,66 @@
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="B5" s="5" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="D5" s="5" t="s">
         <v>174</v>
       </c>
       <c r="E5" s="10" t="s">
+        <v>327</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>328</v>
+      </c>
+      <c r="G5" s="10" t="s">
         <v>329</v>
       </c>
-      <c r="F5" s="10" t="s">
+      <c r="H5" s="10" t="s">
         <v>330</v>
       </c>
-      <c r="G5" s="10" t="s">
-        <v>331</v>
-      </c>
-      <c r="H5" s="10" t="s">
+      <c r="I5" s="10" t="s">
         <v>332</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="J5" s="10" t="s">
+        <v>333</v>
+      </c>
+      <c r="K5" s="10" t="s">
         <v>334</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="L5" s="10" t="s">
         <v>335</v>
       </c>
-      <c r="K5" s="10" t="s">
+      <c r="M5" s="10" t="s">
         <v>336</v>
       </c>
-      <c r="L5" s="10" t="s">
+      <c r="N5" s="10" t="s">
         <v>337</v>
       </c>
-      <c r="M5" s="10" t="s">
+      <c r="O5" s="10" t="s">
         <v>338</v>
       </c>
-      <c r="N5" s="10" t="s">
+      <c r="P5" s="10" t="s">
         <v>339</v>
       </c>
-      <c r="O5" s="10" t="s">
+      <c r="Q5" s="61" t="s">
         <v>340</v>
-      </c>
-      <c r="P5" s="10" t="s">
-        <v>341</v>
-      </c>
-      <c r="Q5" s="61" t="s">
-        <v>342</v>
       </c>
     </row>
     <row r="6" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>509</v>
+        <v>506</v>
       </c>
       <c r="D6" s="6">
         <v>1</v>
@@ -42360,7 +42364,7 @@
       <c r="I6" s="6"/>
       <c r="J6" s="6"/>
       <c r="K6" s="6" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="L6" s="6"/>
       <c r="M6" s="6" t="s">
@@ -42373,13 +42377,13 @@
     </row>
     <row r="7" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="D7" s="6">
         <v>1</v>
@@ -42391,7 +42395,7 @@
       <c r="I7" s="6"/>
       <c r="J7" s="6"/>
       <c r="K7" s="6" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="L7" s="6"/>
       <c r="M7" s="6" t="s">
@@ -42404,13 +42408,13 @@
     </row>
     <row r="8" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="D8" s="6">
         <v>2</v>
@@ -42422,7 +42426,7 @@
       <c r="I8" s="6"/>
       <c r="J8" s="6"/>
       <c r="K8" s="6" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="L8" s="6"/>
       <c r="M8" s="6" t="s">
@@ -42435,13 +42439,13 @@
     </row>
     <row r="9" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="D9" s="6">
         <v>2</v>
@@ -42453,7 +42457,7 @@
       <c r="I9" s="6"/>
       <c r="J9" s="6"/>
       <c r="K9" s="6" t="s">
-        <v>511</v>
+        <v>508</v>
       </c>
       <c r="L9" s="6"/>
       <c r="M9" s="6" t="s">
@@ -44310,37 +44314,37 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="B1" s="22"/>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="73" t="s">
-        <v>325</v>
+        <v>323</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C3" s="46" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="73"/>
       <c r="B4" s="5" t="s">
-        <v>487</v>
+        <v>484</v>
       </c>
       <c r="C4" s="46" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="74"/>
       <c r="B5" s="5" t="s">
-        <v>327</v>
+        <v>325</v>
       </c>
       <c r="C5" s="46" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -44349,7 +44353,7 @@
         <v>174</v>
       </c>
       <c r="C6" s="66" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -44359,40 +44363,40 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="73" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B8" s="10" t="s">
-        <v>329</v>
+        <v>327</v>
       </c>
       <c r="C8" s="46" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="74"/>
       <c r="B9" s="10" t="s">
-        <v>330</v>
+        <v>328</v>
       </c>
       <c r="C9" s="46" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="74"/>
       <c r="B10" s="10" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="C10" s="46" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="13.8" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="74"/>
       <c r="B11" s="10" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="C11" s="57" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -44402,85 +44406,85 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="73" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
       <c r="B13" s="10" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C13" s="46" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="41.4" x14ac:dyDescent="0.25">
       <c r="A14" s="74"/>
       <c r="B14" s="10" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C14" s="46" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="74"/>
       <c r="B15" s="10" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C15" s="46" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="74"/>
       <c r="B16" s="10" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C16" s="46" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="74"/>
       <c r="B17" s="10" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
       <c r="C17" s="46" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="74"/>
       <c r="B18" s="10" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
       <c r="C18" s="46" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="74"/>
       <c r="B19" s="10" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
       <c r="C19" s="46" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="74"/>
       <c r="B20" s="10" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
       <c r="C20" s="46" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="74"/>
       <c r="B21" s="61" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="C21" s="46" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
     </row>
   </sheetData>
@@ -44510,20 +44514,20 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="12" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
       <c r="C4" s="14" t="s">
         <v>187</v>
@@ -44567,7 +44571,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>500</v>
+        <v>497</v>
       </c>
       <c r="C5" s="11" t="s">
         <v>159</v>
@@ -44579,16 +44583,16 @@
         <v>86</v>
       </c>
       <c r="F5" s="11" t="s">
-        <v>512</v>
+        <v>509</v>
       </c>
       <c r="G5" s="11"/>
       <c r="H5" s="11"/>
       <c r="I5" s="11"/>
       <c r="J5" s="11" t="s">
-        <v>513</v>
+        <v>510</v>
       </c>
       <c r="K5" s="11" t="s">
-        <v>514</v>
+        <v>511</v>
       </c>
       <c r="L5" s="11"/>
       <c r="M5" s="11"/>
@@ -44813,7 +44817,7 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="22" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -44821,15 +44825,15 @@
         <v>186</v>
       </c>
       <c r="B3" s="46" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="48" t="s">
-        <v>457</v>
+        <v>454</v>
       </c>
       <c r="B4" s="46" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -44837,7 +44841,7 @@
         <v>187</v>
       </c>
       <c r="B5" s="46" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
@@ -44845,7 +44849,7 @@
         <v>189</v>
       </c>
       <c r="B6" s="46" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="96.6" x14ac:dyDescent="0.25">
@@ -44853,7 +44857,7 @@
         <v>190</v>
       </c>
       <c r="B7" s="46" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
@@ -44861,7 +44865,7 @@
         <v>191</v>
       </c>
       <c r="B8" s="46" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
@@ -44869,7 +44873,7 @@
         <v>188</v>
       </c>
       <c r="B9" s="46" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="55.2" x14ac:dyDescent="0.25">
@@ -44877,7 +44881,7 @@
         <v>192</v>
       </c>
       <c r="B10" s="46" t="s">
-        <v>283</v>
+        <v>281</v>
       </c>
     </row>
     <row r="11" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
@@ -44885,7 +44889,7 @@
         <v>193</v>
       </c>
       <c r="B11" s="46" t="s">
-        <v>284</v>
+        <v>282</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
@@ -44893,7 +44897,7 @@
         <v>194</v>
       </c>
       <c r="B12" s="46" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
@@ -44901,7 +44905,7 @@
         <v>195</v>
       </c>
       <c r="B13" s="46" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
@@ -44909,7 +44913,7 @@
         <v>196</v>
       </c>
       <c r="B14" s="46" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -44917,7 +44921,7 @@
         <v>197</v>
       </c>
       <c r="B15" s="46" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
     </row>
     <row r="16" spans="1:2" ht="27.6" x14ac:dyDescent="0.25">
@@ -44925,7 +44929,7 @@
         <v>199</v>
       </c>
       <c r="B16" s="46" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>

</xml_diff>